<commit_message>
chore(mappings): add example mapping data and metadata files
- Updated `mappings_template.xlsx` with refinements
- Added `scripts/utils/sssom_mapping_data.tsv` containing test mapping rows
- Added `scripts/utils/sssom_mapping_set_metadata.yaml` with:
  - Initiative description, provenance, and licensing info
  - Mapping set identifiers (W3ID, title, description, versioning)
  - CURIE map for prefixes
  - Extension definitions (`replaces`, `isReplacedBy`)
</commit_message>
<xml_diff>
--- a/resources/mappings_template.xlsx
+++ b/resources/mappings_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\semantic-interoperability\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7097BCB-5D19-4C4F-8926-512477EF535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0389B3E-6104-42E6-882F-0889F973D33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>subject_id</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>URI</t>
+  </si>
+  <si>
+    <t>replaces</t>
+  </si>
+  <si>
+    <t>isReplacedBy</t>
+  </si>
+  <si>
+    <t>predicate_modifier</t>
   </si>
 </sst>
 </file>
@@ -112,12 +121,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,13 +147,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -633,29 +698,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:R4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="subject_id" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_label" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="predicate_id" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_id" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="object_label" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="object_category" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="mapping_justification" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="author_id" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="author_label" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="reviewer_id" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="reviewer_label" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="license" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{D5A25AB7-5E38-4BCC-90AC-D512140BE136}" name="subject_type" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{E5DFB3E1-97FD-4961-862A-0DCB3E04A88F}" name="subject_source" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{23A44C72-B578-4829-A5C5-AB470041DD98}" name="subject_source_version" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{2943F8F5-2F20-4295-8400-FE9F9678A588}" name="object_source" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="mapping_date" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{FFDF03DC-B536-477D-9D38-78F1565637A7}" name="comment" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:U4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:U4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
+  <tableColumns count="21">
+    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="subject_id" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_label" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="predicate_id" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="predicate_modifier"/>
+    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_id" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="object_label" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="object_category" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="mapping_justification" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="author_id" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="author_label" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="reviewer_id" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="reviewer_label" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="license" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{D5A25AB7-5E38-4BCC-90AC-D512140BE136}" name="subject_type" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{E5DFB3E1-97FD-4961-862A-0DCB3E04A88F}" name="subject_source" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{23A44C72-B578-4829-A5C5-AB470041DD98}" name="subject_source_version" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{2943F8F5-2F20-4295-8400-FE9F9678A588}" name="object_source" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="mapping_date" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="replaces" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{8856F02D-B0EB-497C-9D58-5A4404049640}" name="isReplacedBy" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="comment" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -990,68 +1058,79 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="15.6328125" customWidth="1"/>
+    <col min="1" max="20" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs(mapping-set): add `object_source_version`; clarify template; fix cardinality glyph; update XLSX
- Add `object_source_version` slot to schema table and provide example
  - Document default in “Defaults” section (latest ontology version, e.g., `1.0.0`)
  - Aligns with SSSOM slot definition (range: String)
- Clarify submission instructions and color-coding of field headers:
  - mandatory (no default): black
  - mandatory (fixed default): purple, pre-filled
  - mandatory (variable default): purple, not pre-filled
  - optional: green
- Normalize contributor column note for `predicate_modifier` (cardinality already indicates optionality)
- Fix mis-encoded cardinality glyph in `mapping_justification` row
- Reposition `comment` row for readability
- Update `resources/mappings_template.xlsx` to reflect new slot and color-coding
- Add TODOs for template defaults and `mapping_date`

Refs: SSSOM `object_source_version` slot (https://mapping-commons.github.io/sssom/object_source_version/)
</commit_message>
<xml_diff>
--- a/resources/mappings_template.xlsx
+++ b/resources/mappings_template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\semantic-interoperability\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0389B3E-6104-42E6-882F-0889F973D33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6006F936-2DC3-43E7-AA20-C04BA0C84087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappings" sheetId="1" r:id="rId1"/>
     <sheet name="Prefixes" sheetId="2" r:id="rId2"/>
+    <sheet name="Hash" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>subject_id</t>
   </si>
@@ -106,13 +107,49 @@
   </si>
   <si>
     <t>predicate_modifier</t>
+  </si>
+  <si>
+    <t>record_id</t>
+  </si>
+  <si>
+    <t>creator_id</t>
+  </si>
+  <si>
+    <t>creator_label</t>
+  </si>
+  <si>
+    <t>object_source_version</t>
+  </si>
+  <si>
+    <t>publication_date</t>
+  </si>
+  <si>
+    <t>Health-RI Semantic Interoperability Initiative</t>
+  </si>
+  <si>
+    <t>https://w3id.org/health-ri/semantic-interoperability</t>
+  </si>
+  <si>
+    <t>HASH</t>
+  </si>
+  <si>
+    <t>semapv:ManualMappingCuration</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>http://w3id.org/health-ri/ontology</t>
+  </si>
+  <si>
+    <t>CRC-32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +157,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +176,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,135 +213,183 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -698,30 +815,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:U4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:U4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
-  <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="subject_id" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_label" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="predicate_id" dataDxfId="17"/>
-    <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="predicate_modifier"/>
-    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_id" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="object_label" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="object_category" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="mapping_justification" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="author_id" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="author_label" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="reviewer_id" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="reviewer_label" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="license" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{D5A25AB7-5E38-4BCC-90AC-D512140BE136}" name="subject_type" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{E5DFB3E1-97FD-4961-862A-0DCB3E04A88F}" name="subject_source" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{23A44C72-B578-4829-A5C5-AB470041DD98}" name="subject_source_version" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{2943F8F5-2F20-4295-8400-FE9F9678A588}" name="object_source" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="mapping_date" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="replaces" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{8856F02D-B0EB-497C-9D58-5A4404049640}" name="isReplacedBy" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="comment" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:Z4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="25">
+  <autoFilter ref="A1:Z4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="23"/>
+    <tableColumn id="24" xr3:uid="{E31C51FF-F9AD-475F-9F4C-5928C1897048}" name="subject_label"/>
+    <tableColumn id="23" xr3:uid="{CE7AF749-7B4B-4226-8150-13024DD6295F}" name="predicate_id"/>
+    <tableColumn id="22" xr3:uid="{D6FFE393-4DC9-49A9-9C9B-0BA6E4351B72}" name="predicate_modifier"/>
+    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="22"/>
+    <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="object_label"/>
+    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="19"/>
+    <tableColumn id="25" xr3:uid="{4D5897AE-98CC-421A-8916-FA23AC9E84FD}" name="author_label"/>
+    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="13"/>
+    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{8856F02D-B0EB-497C-9D58-5A4404049640}" name="object_source" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="5"/>
+    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="4"/>
+    <tableColumn id="30" xr3:uid="{C061BC49-B031-4CB5-B977-9560FD012F56}" name="isReplacedBy" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -735,6 +857,57 @@
     <tableColumn id="2" xr3:uid="{9FD0CC88-7BCF-44DD-917A-4DCFF0710D03}" name="URI"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20FEFA3C-87BD-4761-9EAB-32AE51ADFEC7}" name="Table3" displayName="Table3" ref="A1:Z4" totalsRowShown="0">
+  <autoFilter ref="A1:Z4" xr:uid="{20FEFA3C-87BD-4761-9EAB-32AE51ADFEC7}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{4FDD882A-7228-421A-AA68-F64B4A19C43C}" name="record_id"/>
+    <tableColumn id="2" xr3:uid="{D0AF222F-2301-4B65-8CB4-7706D2873BC0}" name="subject_id"/>
+    <tableColumn id="3" xr3:uid="{D335C766-4703-4450-82BC-371143873D2C}" name="subject_label"/>
+    <tableColumn id="4" xr3:uid="{8DDC1DA9-877C-4868-AF20-25CFB369E074}" name="predicate_id"/>
+    <tableColumn id="5" xr3:uid="{C9D0BF3C-E311-4533-9A0D-BF02475CC0DF}" name="predicate_modifier"/>
+    <tableColumn id="6" xr3:uid="{736DB1AD-7AF7-46CA-A82C-D6B36E8B309A}" name="object_id"/>
+    <tableColumn id="7" xr3:uid="{8E95B2F2-79B4-4DF7-84E3-C9A3B95DAF05}" name="object_label"/>
+    <tableColumn id="8" xr3:uid="{4F13B562-5A39-4A58-ACCD-024F9F21A2BE}" name="object_category"/>
+    <tableColumn id="9" xr3:uid="{F263EFF9-54C4-43DF-B814-398CEFDA72D4}" name="mapping_justification"/>
+    <tableColumn id="10" xr3:uid="{E1F915B8-8E9D-4F6E-AF3D-53E5238EE408}" name="author_id"/>
+    <tableColumn id="11" xr3:uid="{001B78BB-DE8D-41BE-BCC4-D934297A6CEC}" name="author_label"/>
+    <tableColumn id="12" xr3:uid="{6D4EAC80-1AD8-4056-B80C-C5EE7D842D08}" name="reviewer_id"/>
+    <tableColumn id="13" xr3:uid="{7428200C-BD5D-4596-99BC-13F516330D58}" name="reviewer_label"/>
+    <tableColumn id="14" xr3:uid="{7A3A1692-9BD0-4019-AE48-817739D25975}" name="creator_id"/>
+    <tableColumn id="15" xr3:uid="{F346F4A4-2913-4494-9BBC-38739A8033F5}" name="creator_label"/>
+    <tableColumn id="16" xr3:uid="{9527D45B-717F-4888-9B86-A55EFAADDEDB}" name="license"/>
+    <tableColumn id="17" xr3:uid="{D4B4B6DB-1EEF-4C0E-AFB8-A0CA0BD3DB99}" name="subject_type"/>
+    <tableColumn id="18" xr3:uid="{1372EBD2-4399-4621-90B1-3130F25B9371}" name="subject_source"/>
+    <tableColumn id="19" xr3:uid="{7266452A-F272-43F4-BA27-03EF40AEA97B}" name="subject_source_version"/>
+    <tableColumn id="20" xr3:uid="{3C897F60-B0FA-478D-8C90-C23A6D3E3520}" name="object_source"/>
+    <tableColumn id="21" xr3:uid="{BC303C80-F7DB-47AA-AA8B-4EFAB06C137E}" name="object_source_version"/>
+    <tableColumn id="22" xr3:uid="{495885EF-F462-4CEB-BE9F-5E8694B5F395}" name="mapping_date"/>
+    <tableColumn id="23" xr3:uid="{93DC2089-463F-4BB1-B95C-5108C64D5D3B}" name="publication_date"/>
+    <tableColumn id="24" xr3:uid="{520812E4-78A0-4E07-BD50-3994D98373BA}" name="comment"/>
+    <tableColumn id="25" xr3:uid="{DF632399-E8ED-4E1E-AB38-879DE81879EF}" name="replaces"/>
+    <tableColumn id="26" xr3:uid="{914433F2-8EE3-4CCE-A6A3-C542F570EF87}" name="isReplacedBy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}" name="Table4" displayName="Table4" ref="AB1:AD4" totalsRowShown="0">
+  <autoFilter ref="AB1:AD4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="1">
+      <calculatedColumnFormula>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1058,81 +1231,166 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" t="s">
+        <v>33</v>
+      </c>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1150,17 +1408,15 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="55.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1174,4 +1430,151 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB0CEB3-7F06-4536-AFD2-9DCFD59FAD1D}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:AD4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="26" width="10.7109375" customWidth="1"/>
+    <col min="28" max="30" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB2" t="str">
+        <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
+        <v/>
+      </c>
+      <c r="AC2" s="10"/>
+      <c r="AD2" t="str">
+        <f>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</f>
+        <v>hrim:</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB3" t="str">
+        <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
+        <v/>
+      </c>
+      <c r="AC3" s="10"/>
+      <c r="AD3" t="str">
+        <f>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</f>
+        <v>hrim:</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB4" t="str">
+        <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
+        <v/>
+      </c>
+      <c r="AC4" s="10"/>
+      <c r="AD4" t="str">
+        <f>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</f>
+        <v>hrim:</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore(resources): update mappings_template.xlsx to align columns with latest SSSOM definitions
- revise column set and ordering to match current spec
- refresh headers/notes and in-sheet guidance for contributors
</commit_message>
<xml_diff>
--- a/resources/mappings_template.xlsx
+++ b/resources/mappings_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\semantic-interoperability\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6006F936-2DC3-43E7-AA20-C04BA0C84087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2B62E-A067-4FCB-AEBF-42DDBEE77384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappings" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>subject_id</t>
   </si>
@@ -85,9 +85,6 @@
     <t>subject_source_version</t>
   </si>
   <si>
-    <t>object_source</t>
-  </si>
-  <si>
     <t>mapping_date</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>replaces</t>
   </si>
   <si>
-    <t>isReplacedBy</t>
-  </si>
-  <si>
     <t>predicate_modifier</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by/4.0/</t>
-  </si>
-  <si>
-    <t>http://w3id.org/health-ri/ontology</t>
   </si>
   <si>
     <t>CRC-32</t>
@@ -217,24 +208,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -247,7 +336,268 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -390,414 +740,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -815,35 +757,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:Z4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="25">
-  <autoFilter ref="A1:Z4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
-  <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:X4" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:X4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="20"/>
     <tableColumn id="24" xr3:uid="{E31C51FF-F9AD-475F-9F4C-5928C1897048}" name="subject_label"/>
     <tableColumn id="23" xr3:uid="{CE7AF749-7B4B-4226-8150-13024DD6295F}" name="predicate_id"/>
     <tableColumn id="22" xr3:uid="{D6FFE393-4DC9-49A9-9C9B-0BA6E4351B72}" name="predicate_modifier"/>
-    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="19"/>
     <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="object_label"/>
-    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="16"/>
     <tableColumn id="25" xr3:uid="{4D5897AE-98CC-421A-8916-FA23AC9E84FD}" name="author_label"/>
-    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{8856F02D-B0EB-497C-9D58-5A4404049640}" name="object_source" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="9"/>
-    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="5"/>
-    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="4"/>
-    <tableColumn id="30" xr3:uid="{C061BC49-B031-4CB5-B977-9560FD012F56}" name="isReplacedBy" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="8"/>
+    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="3"/>
+    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="2"/>
+    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="0"/>
+    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="1"/>
+    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -861,9 +801,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20FEFA3C-87BD-4761-9EAB-32AE51ADFEC7}" name="Table3" displayName="Table3" ref="A1:Z4" totalsRowShown="0">
-  <autoFilter ref="A1:Z4" xr:uid="{20FEFA3C-87BD-4761-9EAB-32AE51ADFEC7}"/>
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20FEFA3C-87BD-4761-9EAB-32AE51ADFEC7}" name="Table3" displayName="Table3" ref="A1:X4" totalsRowShown="0">
+  <autoFilter ref="A1:X4" xr:uid="{20FEFA3C-87BD-4761-9EAB-32AE51ADFEC7}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{4FDD882A-7228-421A-AA68-F64B4A19C43C}" name="record_id"/>
     <tableColumn id="2" xr3:uid="{D0AF222F-2301-4B65-8CB4-7706D2873BC0}" name="subject_id"/>
     <tableColumn id="3" xr3:uid="{D335C766-4703-4450-82BC-371143873D2C}" name="subject_label"/>
@@ -883,27 +823,25 @@
     <tableColumn id="17" xr3:uid="{D4B4B6DB-1EEF-4C0E-AFB8-A0CA0BD3DB99}" name="subject_type"/>
     <tableColumn id="18" xr3:uid="{1372EBD2-4399-4621-90B1-3130F25B9371}" name="subject_source"/>
     <tableColumn id="19" xr3:uid="{7266452A-F272-43F4-BA27-03EF40AEA97B}" name="subject_source_version"/>
-    <tableColumn id="20" xr3:uid="{3C897F60-B0FA-478D-8C90-C23A6D3E3520}" name="object_source"/>
     <tableColumn id="21" xr3:uid="{BC303C80-F7DB-47AA-AA8B-4EFAB06C137E}" name="object_source_version"/>
     <tableColumn id="22" xr3:uid="{495885EF-F462-4CEB-BE9F-5E8694B5F395}" name="mapping_date"/>
     <tableColumn id="23" xr3:uid="{93DC2089-463F-4BB1-B95C-5108C64D5D3B}" name="publication_date"/>
     <tableColumn id="24" xr3:uid="{520812E4-78A0-4E07-BD50-3994D98373BA}" name="comment"/>
     <tableColumn id="25" xr3:uid="{DF632399-E8ED-4E1E-AB38-879DE81879EF}" name="replaces"/>
-    <tableColumn id="26" xr3:uid="{914433F2-8EE3-4CCE-A6A3-C542F570EF87}" name="isReplacedBy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}" name="Table4" displayName="Table4" ref="AB1:AD4" totalsRowShown="0">
-  <autoFilter ref="AB1:AD4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}" name="Table4" displayName="Table4" ref="Z1:AB4" totalsRowShown="0">
+  <autoFilter ref="Z1:AB4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="6">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="4">
       <calculatedColumnFormula>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1231,166 +1169,142 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7265625" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="30.7265625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>23</v>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
+      <c r="E1" t="s">
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="U1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>21</v>
+      <c r="X1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="G2" s="2"/>
       <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" t="s">
-        <v>33</v>
-      </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1410,18 +1324,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="55.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1437,19 +1351,19 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="26" width="10.7109375" customWidth="1"/>
-    <col min="28" max="30" width="15.7109375" customWidth="1"/>
+    <col min="1" max="24" width="10.7265625" customWidth="1"/>
+    <col min="26" max="28" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1461,7 +1375,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -1472,7 +1386,7 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1488,10 +1402,10 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s">
         <v>11</v>
@@ -1506,65 +1420,59 @@
         <v>14</v>
       </c>
       <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
-        <v>27</v>
-      </c>
       <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AB2" t="str">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="Z2" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
         <v/>
       </c>
-      <c r="AC2" s="10"/>
-      <c r="AD2" t="str">
+      <c r="AA2" s="6"/>
+      <c r="AB2" t="str">
         <f>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</f>
         <v>hrim:</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AB3" t="str">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="Z3" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
         <v/>
       </c>
-      <c r="AC3" s="10"/>
-      <c r="AD3" t="str">
+      <c r="AA3" s="6"/>
+      <c r="AB3" t="str">
         <f>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</f>
         <v>hrim:</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AB4" t="str">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="Z4" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
         <v/>
       </c>
-      <c r="AC4" s="10"/>
-      <c r="AD4" t="str">
+      <c r="AA4" s="6"/>
+      <c r="AB4" t="str">
         <f>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</f>
         <v>hrim:</v>
       </c>

</xml_diff>

<commit_message>
docs(news): linkify and expand 2025-11-03 entries; feat(template): add basic input validation and contextual info
- news.md:
  - Linkify page titles and expand 2025-11-03 bullets (Mapping Set, Mapping Strategy, Mappings Template).
  - Merge Mapping Set changes into a single concise line (HTTPS examples, predicate_id allowed values, remove default object_source, etc.).
- mappings_template.xlsx:
  - Add basic input validation and show contextual info when boxes are selected.

Files:
- docs/news.md
- resources/mappings_template.xlsx
</commit_message>
<xml_diff>
--- a/resources/mappings_template.xlsx
+++ b/resources/mappings_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\semantic-interoperability\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2B62E-A067-4FCB-AEBF-42DDBEE77384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F77EAE-935C-449B-99F4-0F9A3493911A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappings" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,85 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFEB9C"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9C5700"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -265,30 +343,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -322,6 +376,390 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -334,417 +772,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFEB9C"/>
+      <color rgb="FF9C5700"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -762,11 +798,11 @@
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="20"/>
-    <tableColumn id="24" xr3:uid="{E31C51FF-F9AD-475F-9F4C-5928C1897048}" name="subject_label"/>
+    <tableColumn id="24" xr3:uid="{E31C51FF-F9AD-475F-9F4C-5928C1897048}" name="subject_label" dataCellStyle="Normal"/>
     <tableColumn id="23" xr3:uid="{CE7AF749-7B4B-4226-8150-13024DD6295F}" name="predicate_id"/>
     <tableColumn id="22" xr3:uid="{D6FFE393-4DC9-49A9-9C9B-0BA6E4351B72}" name="predicate_modifier"/>
     <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="object_label"/>
+    <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="object_label" dataCellStyle="Normal"/>
     <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="18"/>
     <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="17"/>
     <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="16"/>
@@ -779,11 +815,11 @@
     <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="10"/>
     <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="9"/>
     <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="3"/>
-    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="2"/>
-    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="0"/>
-    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,11 +873,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}" name="Table4" displayName="Table4" ref="Z1:AB4" totalsRowShown="0">
   <autoFilter ref="Z1:AB4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="24">
       <calculatedColumnFormula>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1172,17 +1208,18 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="30.7265625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="30.7265625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="14" max="15" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="30.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -1216,7 +1253,7 @@
       <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M1" t="s">
@@ -1256,9 +1293,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="G2" s="2"/>
       <c r="I2" t="s">
         <v>29</v>
       </c>
@@ -1274,7 +1310,7 @@
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I3" t="s">
         <v>29</v>
       </c>
@@ -1290,7 +1326,7 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
         <v>29</v>
       </c>
@@ -1307,6 +1343,65 @@
       <c r="V4" s="7"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D4">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="narrower">
+      <formula>NOT(ISERROR(SEARCH("narrower",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="broader">
+      <formula>NOT(ISERROR(SEARCH("broader",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="exact">
+      <formula>NOT(ISERROR(SEARCH("exact",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid predicate_modifier" error="Leave blank or set to Not (case-sensitive). No other values allowed." promptTitle="About predicate_modifier" prompt="Optional. Leave blank or set to Not to negate the predicate." sqref="E2:E4" xr:uid="{E9C6CA8F-7B41-4974-A5B0-AF180B53928D}">
+      <formula1>"Not"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid object_id" error="Enter a CURIE using a bound prefix (e.g., hrio:Person) or an absolute HTTP(S) URI." promptTitle="About object_id" prompt="Required. CURIE with a bound prefix (e.g., hrio:Person) or absolute HTTP(S) URI." sqref="F2:F4" xr:uid="{C7BA574B-58BE-4B14-BCEB-EE209EEA940D}">
+      <formula1>AND(ISNUMBER(FIND(":", F2)), FIND(":", F2) &gt; 1, FIND(":", F2) &lt; LEN(F2))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid predicate_id" error="Choose one of: hriv:hasExactMeaning | hriv:hasBroaderMeaningThan | hriv:hasNarrowerMeaningThan." promptTitle="About predicate_id" prompt="Required. Choose one: hriv:hasExactMeaning | hriv:hasBroaderMeaningThan | hriv:hasNarrowerMeaningThan." sqref="D2:D4" xr:uid="{EE3A1558-2E21-469A-A555-9CD140B407FE}">
+      <formula1>"hriv:hasExactMeaning,hriv:hasBroaderMeaningThan,hriv:hasNarrowerMeaningThan"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid subject_label" error="If provided, use a language-tagged label: text@lang (BCP 47). Examples: Patient@en, Patiënt@nl." promptTitle="About subject_label" prompt="Optional. Language-tagged label text@lang (BCP 47). Examples: Patient@en, Patiënt@nl." sqref="C2:C4" xr:uid="{8FAEF3FD-962D-4142-9C91-4A6BF14FA3C9}">
+      <formula1>AND(ISNUMBER(FIND("@", C2)), FIND("@", C2) &gt; 1, FIND("@", C2) &lt; LEN(C2))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid object_category" error="If provided, enter a valid OntoUML stereotype (e.g., kind, role, phase)." promptTitle="About object_category" prompt="Optional. OntoUML stereotype of the object, e.g., kind, role, phase." sqref="H2:H4" xr:uid="{39BC81D8-B6DA-4A18-8966-20D2F9D986DF}">
+      <formula1>"abstract,category,collective,datatype,enumeration,event,historicalRole,historicalRoleMixin,kind,mixin,mode,phase,phaseMixin,quality,quantity,relator,role,roleMixin,situation,subkind,type"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid object_label" error="If provided, use a language-tagged label: text@lang (BCP 47). Example: Person@en." promptTitle="About object_label" prompt="Optional. Language-tagged label text@lang (BCP 47). Example: Person@en." sqref="G2:G4" xr:uid="{4125C845-9C29-4C7B-AAC6-E9A212DEE6F9}">
+      <formula1>AND(ISNUMBER(FIND("@", G2)), FIND("@", G2) &gt; 1, FIND("@", G2) &lt; LEN(G2))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid justification" error="Use semapv:ManualMappingCuration (unless otherwise instructed by curators)." promptTitle="About justification" prompt="Required. Use semapv:ManualMappingCuration (default)." sqref="I2:I4" xr:uid="{85C98ED9-F335-4EF0-8173-F72FEB9981BB}">
+      <formula1>"semapv:ManualMappingCuration"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid subject_source" error="If provided, enter the source vocabulary as CURIE/URI (e.g., https://hl7.org/fhir)." promptTitle="About subject_source" prompt="Optional. Source vocabulary as CURIE/URI, e.g., https://hl7.org/fhir." sqref="R2:R4" xr:uid="{3DD665BE-4401-44FA-B719-9946EE2B6E52}">
+      <formula1>AND(ISNUMBER(FIND(":", R2)), FIND(":", R2) &gt; 1, FIND(":", R2) &lt; LEN(R2))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="About license" prompt="Required. Absolute HTTP(S) URL. Default: https://creativecommons.org/licenses/by/4.0/." sqref="P2:P4" xr:uid="{B8B406B1-7163-4511-AF2A-82A6E580C4A4}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid subject_type" error="If provided, use an SSSOM EntityTypeEnum value (e.g., owl class, rdf property)." promptTitle="About subject_type" prompt="Optional. SSSOM EntityTypeEnum value, e.g., owl class, rdf property." sqref="Q2:Q4" xr:uid="{AFD48CE2-264C-4EB8-8757-118A4663D391}">
+      <formula1>"owl class,owl object property,owl data property,owl annotation property,owl named individual,skos concept,rdfs resource,rdfs class,rdfs literal,rdfs datatype,rdf property,composed entity expression"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid HRIO version" error="If provided, enter the HRIO version (e.g., 1.0.0). Avoid leading/trailing spaces." promptTitle="About object_source_version" prompt="Optional. HRIO version used, e.g., 1.0.0. Defaults to the latest if omitted." sqref="T2:T4" xr:uid="{6ABC9030-E066-4774-9BE6-CE9355570CB3}">
+      <formula1>AND(LEN(T2)-LEN(SUBSTITUTE(T2, ".", "")) = 2, ISNUMBER(VALUE(SUBSTITUTE(T2, ".", ""))))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid mapping_date" error="Enter a date in YYYY-MM-DD (ISO 8601). Must be a valid calendar date." promptTitle="About mapping_date" prompt="Required. Date the mapping was created. Format: YYYY-MM-DD." sqref="U2:U4" xr:uid="{C8B92F9B-BF7F-48B7-8FA8-D0901722454C}">
+      <formula1>AND(LEN(U2)=10, MID(U2, 5, 1)="-", MID(U2, 8, 1)="-", ISNUMBER(DATEVALUE(U2)))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid subject_id" error="Enter a CURIE using a bound prefix from the Prefixes sheet (e.g., fhir:Patient) or an absolute HTTP(S) URI." promptTitle="About subject_id" prompt="Required. CURIE with a bound prefix (see Prefixes) or absolute HTTP(S) URI. Example: fhir:Patient." sqref="B2:B4" xr:uid="{A26CDB3D-1F19-4BBD-8A0B-C182F97FFA2C}">
+      <formula1>AND(ISNUMBER(FIND(":", B2)), FIND(":", B2) &gt; 1, FIND(":", B2) &lt; LEN(B2))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid author_id" error="Enter one or more IDs as CURIE/URI. Separate multiple with a comma." promptTitle="About author_id" prompt="Required (1+). CURIE/URI identifiers. Separate multiple with a comma." sqref="J2:J4" xr:uid="{2706DD3F-E508-4F6B-8CD3-D471ADD6DB78}">
+      <formula1>AND(ISNUMBER(FIND(":", J2)), FIND(":", J2) &gt; 1, FIND(":", J2) &lt; LEN(J2))</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid reviewer_id" error="Enter at least one reviewer ID as CURIE/URI. Separate multiple with a comma." promptTitle="About reviewer_id" prompt="Required (1+). Reviewer IDs as CURIE/URI. Separate multiple with a comma." sqref="L2:L4" xr:uid="{8E8DE317-C421-4E46-8C08-5E463CA92743}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid reviewer_label" error="If provided, enter one or more names. Separate multiple with a comma." promptTitle="About reviewer_label" prompt="Optional (1+). Reviewer names. Separate multiple with a comma." sqref="M2:M4" xr:uid="{A7AE094B-0622-41B2-BBD4-43E96682640B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="subject source version" prompt="Optional. Version of the subject source, e.g., R4." sqref="S2:S4" xr:uid="{36411772-3817-47EB-94F8-6793649DB90E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid author_label" error="If provided, enter one or more names. Separate multiple with a comma." promptTitle="About author_label" prompt="Optional (1+). Author names. Separate multiple with a comma." sqref="K2:K4" xr:uid="{753276A0-496D-463B-A30F-7FDAA894DA31}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="About comment" prompt="Optional. Short free-text note. Keep concise; plain text only." sqref="W2:W4" xr:uid="{96C51DCA-76FA-4D4A-AD5E-5421C5CC1FD8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="About replaces" prompt="Optional (0..*). Record URI(s) that this entry replaces. Separate multiple with `" sqref="X2:X4" xr:uid="{86C8DF89-AEAC-40A6-BCF3-FB06F5CB6713}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -1322,15 +1417,17 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="55.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1339,6 +1436,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{379FEBE4-82E4-4B17-8CE7-0993F7A22FA6}">
+      <formula1>AND(ISNUMBER(FIND(":", B2)), FIND(":", B2) &gt; 1, FIND(":", B2) &lt; LEN(B2))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1355,13 +1457,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="24" width="10.7265625" customWidth="1"/>
-    <col min="26" max="28" width="15.7265625" customWidth="1"/>
+    <col min="1" max="24" width="10.7109375" customWidth="1"/>
+    <col min="26" max="28" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1444,7 +1546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Z2" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
         <v/>
@@ -1455,7 +1557,7 @@
         <v>hrim:</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Z3" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
         <v/>
@@ -1466,7 +1568,7 @@
         <v>hrim:</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Z4" t="str">
         <f>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</f>
         <v/>

</xml_diff>

<commit_message>
chore(resources): refine mappings_template.xlsx colors, rules, and messages
- Adjust cell coloring to match field categories (mandatory, defaulted, optional) for quicker scanning.
- Tighten validation rules to reduce false entries.
- Clarify input tooltips and error texts for contributors (short, action-oriented phrasing).
- No functional changes to schema; improves usability and data quality of submissions.
</commit_message>
<xml_diff>
--- a/resources/mappings_template.xlsx
+++ b/resources/mappings_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\semantic-interoperability\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F77EAE-935C-449B-99F4-0F9A3493911A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46952F9-6487-4050-9E9C-C7A11F6A25D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
   </bookViews>
@@ -222,7 +222,24 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -245,13 +262,74 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFFFEB9C"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF9C5700"/>
-        </patternFill>
-      </fill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9F9F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -758,25 +836,13 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9F9F"/>
+      <color rgb="FFFFE1E1"/>
       <color rgb="FFFFEB9C"/>
       <color rgb="FF9C5700"/>
     </mruColors>
@@ -793,33 +859,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:X4" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:X4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:X4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="30"/>
     <tableColumn id="24" xr3:uid="{E31C51FF-F9AD-475F-9F4C-5928C1897048}" name="subject_label" dataCellStyle="Normal"/>
     <tableColumn id="23" xr3:uid="{CE7AF749-7B4B-4226-8150-13024DD6295F}" name="predicate_id"/>
     <tableColumn id="22" xr3:uid="{D6FFE393-4DC9-49A9-9C9B-0BA6E4351B72}" name="predicate_modifier"/>
-    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="29"/>
     <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="object_label" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="26"/>
     <tableColumn id="25" xr3:uid="{4D5897AE-98CC-421A-8916-FA23AC9E84FD}" name="author_label"/>
-    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="4"/>
-    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="19"/>
+    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="17"/>
+    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="16"/>
+    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="15"/>
+    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="14"/>
+    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -873,11 +939,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}" name="Table4" displayName="Table4" ref="Z1:AB4" totalsRowShown="0">
   <autoFilter ref="Z1:AB4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="10">
       <calculatedColumnFormula>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1344,22 +1410,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="narrower">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="narrower">
       <formula>NOT(ISERROR(SEARCH("narrower",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="broader">
+    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="broader">
       <formula>NOT(ISERROR(SEARCH("broader",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="exact">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="exact">
       <formula>NOT(ISERROR(SEARCH("exact",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="not">
+      <formula>NOT(ISERROR(SEARCH("not",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B4 D2:D4 F2:F4 J2:J4 L2:L4">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
+      <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="20">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid predicate_modifier" error="Leave blank or set to Not (case-sensitive). No other values allowed." promptTitle="About predicate_modifier" prompt="Optional. Leave blank or set to Not to negate the predicate." sqref="E2:E4" xr:uid="{E9C6CA8F-7B41-4974-A5B0-AF180B53928D}">
       <formula1>"Not"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid object_id" error="Enter a CURIE using a bound prefix (e.g., hrio:Person) or an absolute HTTP(S) URI." promptTitle="About object_id" prompt="Required. CURIE with a bound prefix (e.g., hrio:Person) or absolute HTTP(S) URI." sqref="F2:F4" xr:uid="{C7BA574B-58BE-4B14-BCEB-EE209EEA940D}">
-      <formula1>AND(ISNUMBER(FIND(":", F2)), FIND(":", F2) &gt; 1, FIND(":", F2) &lt; LEN(F2))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid object_id" error="Enter a CURIE for a HRIO concept (e.g., hrio:Person)." promptTitle="About object_id" prompt="Enter a CURIE for a HRIO concept (e.g., hrio:Person)." sqref="F2:F4" xr:uid="{C7BA574B-58BE-4B14-BCEB-EE209EEA940D}">
+      <formula1>AND(ISNUMBER(FIND("hrio:", F2)), FIND("hrio:", F2) &gt; 1, FIND("hrio:", F2) &lt; LEN(F2))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid predicate_id" error="Choose one of: hriv:hasExactMeaning | hriv:hasBroaderMeaningThan | hriv:hasNarrowerMeaningThan." promptTitle="About predicate_id" prompt="Required. Choose one: hriv:hasExactMeaning | hriv:hasBroaderMeaningThan | hriv:hasNarrowerMeaningThan." sqref="D2:D4" xr:uid="{EE3A1558-2E21-469A-A555-9CD140B407FE}">
       <formula1>"hriv:hasExactMeaning,hriv:hasBroaderMeaningThan,hriv:hasNarrowerMeaningThan"</formula1>

</xml_diff>

<commit_message>
fix(xlsx): enforce case-sensitive "hrio:" prefix with non-empty suffix in data validation
Update data validation in `resources/mappings_template.xlsx` to require inputs to start with the exact, case-sensitive prefix `hrio:` and include at least one character after it.

Impact: entries lacking the prefix or using the wrong case (e.g., `HRIO:`) are now rejected; incomplete values like `hrio:` alone are blocked.
</commit_message>
<xml_diff>
--- a/resources/mappings_template.xlsx
+++ b/resources/mappings_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroPauloFavatoBarc\Dev\semantic-interoperability\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46952F9-6487-4050-9E9C-C7A11F6A25D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F706728F-8092-4787-8AA1-4A630632A84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1364C1B-3702-4249-8DB4-2D82861A95E3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>subject_id</t>
   </si>
@@ -134,6 +134,54 @@
   </si>
   <si>
     <t>CRC-32</t>
+  </si>
+  <si>
+    <t>dcterms</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/</t>
+  </si>
+  <si>
+    <t>hrim</t>
+  </si>
+  <si>
+    <t>https://w3id.org/health-ri/semantic-interoperability/mappings#</t>
+  </si>
+  <si>
+    <t>hrio</t>
+  </si>
+  <si>
+    <t>https://w3id.org/health-ri/ontology#</t>
+  </si>
+  <si>
+    <t>hriv</t>
+  </si>
+  <si>
+    <t>https://w3id.org/health-ri/mapping-vocabulary#</t>
+  </si>
+  <si>
+    <t>onz-g</t>
+  </si>
+  <si>
+    <t>http://purl.org/ozo/onz-g#</t>
+  </si>
+  <si>
+    <t>orcid</t>
+  </si>
+  <si>
+    <t>https://orcid.org/</t>
+  </si>
+  <si>
+    <t>semapv</t>
+  </si>
+  <si>
+    <t>https://w3id.org/semapv/vocab/</t>
+  </si>
+  <si>
+    <t>sssom</t>
+  </si>
+  <si>
+    <t>https://w3id.org/sssom/</t>
   </si>
 </sst>
 </file>
@@ -222,14 +270,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1E1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -274,46 +315,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF9F9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -859,41 +860,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:X4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}" name="Table1" displayName="Table1" ref="A1:X4" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:X4" xr:uid="{F3A1F876-3ACD-4118-8509-5D77BAD95681}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{418DF1C6-46AE-4D05-8CFD-E9533A5BC2B0}" name="record_id" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{5629DEAA-C64A-4C26-9C3D-441AA1987215}" name="subject_id" dataDxfId="25"/>
     <tableColumn id="24" xr3:uid="{E31C51FF-F9AD-475F-9F4C-5928C1897048}" name="subject_label" dataCellStyle="Normal"/>
     <tableColumn id="23" xr3:uid="{CE7AF749-7B4B-4226-8150-13024DD6295F}" name="predicate_id"/>
     <tableColumn id="22" xr3:uid="{D6FFE393-4DC9-49A9-9C9B-0BA6E4351B72}" name="predicate_modifier"/>
-    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5DE55A22-49F3-4CE4-92AB-E4082CDB5810}" name="object_id" dataDxfId="24"/>
     <tableColumn id="18" xr3:uid="{F897D13D-6D73-46AE-91CB-FF641F299710}" name="object_label" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{0A81517D-DEC8-44BF-8F85-5FF7FE98F200}" name="object_category" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{26DBBA81-542B-4F93-83EE-28068E94BE05}" name="mapping_justification" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{1A470CAB-4A9A-4541-AE74-B2B9A03DD29E}" name="author_id" dataDxfId="21"/>
     <tableColumn id="25" xr3:uid="{4D5897AE-98CC-421A-8916-FA23AC9E84FD}" name="author_label"/>
-    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="19"/>
-    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="18"/>
-    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="15"/>
-    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="14"/>
-    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{DF2F500D-9154-4455-B03E-CC2B6739AE84}" name="reviewer_id" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{499DBD21-2B5A-4A38-9FFA-0477EF18EC6A}" name="reviewer_label" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{72FCD242-C99E-40FF-9358-9CCD02E5EDFA}" name="creator_id" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{899C370E-BA5B-4C4B-927A-CFBD3F409FDE}" name="creator_label" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{F6634A69-4617-4282-808A-1A99C1B24438}" name="license" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{3D7D04A3-334E-46BD-A964-B3690AA2C5D6}" name="subject_type" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{CBE26A85-1268-4A70-B764-04D3EDB43906}" name="subject_source" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{70B1F6AC-3F94-482D-8586-7E477F4E47BE}" name="subject_source_version" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{D429941D-58EA-4400-8BD7-CF5541B8B709}" name="object_source_version" dataDxfId="12"/>
+    <tableColumn id="26" xr3:uid="{8683B23B-85C0-4581-9D45-264D7BAE8FEE}" name="mapping_date" dataDxfId="11"/>
+    <tableColumn id="27" xr3:uid="{92D3255A-1ACB-4AE8-A5F9-358B77734284}" name="publication_date" dataDxfId="10"/>
+    <tableColumn id="28" xr3:uid="{5154C138-4F05-4AD2-81D2-9BB957CAFC21}" name="comment" dataDxfId="9"/>
+    <tableColumn id="29" xr3:uid="{8922DC1B-E4F4-4E06-9EF7-B4ADE68C21FE}" name="replaces" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB1467CD-C73D-4100-B5C5-5FDBC07F3BC9}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{CB1467CD-C73D-4100-B5C5-5FDBC07F3BC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB1467CD-C73D-4100-B5C5-5FDBC07F3BC9}" name="Table2" displayName="Table2" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{CB1467CD-C73D-4100-B5C5-5FDBC07F3BC9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{BC5BD901-C15C-4659-ACC7-AE3A02A88257}" name="Prefix"/>
     <tableColumn id="2" xr3:uid="{9FD0CC88-7BCF-44DD-917A-4DCFF0710D03}" name="URI"/>
@@ -939,11 +940,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}" name="Table4" displayName="Table4" ref="Z1:AB4" totalsRowShown="0">
   <autoFilter ref="Z1:AB4" xr:uid="{DC187EFA-DC60-4013-96D7-B4A7452B0918}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{5C1F10EC-45AF-4A89-B63A-8325F9C5D0CE}" name="HASH" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[mapping_date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{40455983-5BAF-4A79-A2C8-800C9F6F5778}" name="CRC-32" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DDBD3CA0-1C5A-4027-AA34-B67FEEF353D2}" name="record_id" dataDxfId="5">
       <calculatedColumnFormula>"hrim:"&amp;Table4[[#This Row],[CRC-32]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1274,7 +1275,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,25 +1410,25 @@
       <c r="V4" s="7"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D4 B2:B4 F2:F4 J2:J4 L2:L4">
+    <cfRule type="containsBlanks" dxfId="4" priority="7">
+      <formula>LEN(TRIM(B2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="narrower">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="narrower">
       <formula>NOT(ISERROR(SEARCH("narrower",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="broader">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="broader">
       <formula>NOT(ISERROR(SEARCH("broader",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="exact">
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="exact">
       <formula>NOT(ISERROR(SEARCH("exact",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="not">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="not">
       <formula>NOT(ISERROR(SEARCH("not",E2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B4 D2:D4 F2:F4 J2:J4 L2:L4">
-    <cfRule type="containsBlanks" dxfId="5" priority="7">
-      <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="20">
@@ -1435,7 +1436,7 @@
       <formula1>"Not"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid object_id" error="Enter a CURIE for a HRIO concept (e.g., hrio:Person)." promptTitle="About object_id" prompt="Enter a CURIE for a HRIO concept (e.g., hrio:Person)." sqref="F2:F4" xr:uid="{C7BA574B-58BE-4B14-BCEB-EE209EEA940D}">
-      <formula1>AND(ISNUMBER(FIND("hrio:", F2)), FIND("hrio:", F2) &gt; 1, FIND("hrio:", F2) &lt; LEN(F2))</formula1>
+      <formula1>AND(EXACT(LEFT(F2,5),"hrio:"), LEN(F2)&gt;5)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid predicate_id" error="Choose one of: hriv:hasExactMeaning | hriv:hasBroaderMeaningThan | hriv:hasNarrowerMeaningThan." promptTitle="About predicate_id" prompt="Required. Choose one: hriv:hasExactMeaning | hriv:hasBroaderMeaningThan | hriv:hasNarrowerMeaningThan." sqref="D2:D4" xr:uid="{EE3A1558-2E21-469A-A555-9CD140B407FE}">
       <formula1>"hriv:hasExactMeaning,hriv:hasBroaderMeaningThan,hriv:hasNarrowerMeaningThan"</formula1>
@@ -1491,16 +1492,14 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1511,15 +1510,80 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{379FEBE4-82E4-4B17-8CE7-0993F7A22FA6}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{379FEBE4-82E4-4B17-8CE7-0993F7A22FA6}">
       <formula1>AND(ISNUMBER(FIND(":", B2)), FIND(":", B2) &gt; 1, FIND(":", B2) &lt; LEN(B2))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>